<commit_message>
environment changed to production
</commit_message>
<xml_diff>
--- a/IssueTracker.xlsx
+++ b/IssueTracker.xlsx
@@ -10,6 +10,9 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$E$22</definedName>
+  </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -20,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="41">
   <si>
     <t xml:space="preserve">#</t>
   </si>
@@ -40,21 +43,24 @@
     <t xml:space="preserve">/login when manually entered, app must redirect to dashboard if user is already logged in.</t>
   </si>
   <si>
+    <t xml:space="preserve">Open</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reopened for new app.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Auto login – Use of cookies</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Auto logout</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lazy loading for expenses, dashboard and authentication</t>
+  </si>
+  <si>
     <t xml:space="preserve">Closed</t>
   </si>
   <si>
-    <t xml:space="preserve">Auto login – Use of cookies</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Auto logout</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Auto logout should work on the logic of expiration time of token.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lazy loading for expenses, dashboard and authentication</t>
-  </si>
-  <si>
     <t xml:space="preserve">Already done</t>
   </si>
   <si>
@@ -70,9 +76,6 @@
     <t xml:space="preserve">Modulerize whole project</t>
   </si>
   <si>
-    <t xml:space="preserve">Open</t>
-  </si>
-  <si>
     <t xml:space="preserve">In the database there are some blank documents created. </t>
   </si>
   <si>
@@ -95,9 +98,6 @@
   </si>
   <si>
     <t xml:space="preserve">Expenses for January not reflecting in the graph</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Resolved</t>
   </si>
   <si>
     <t xml:space="preserve">Updated in the new version, yet to be pushed and deployed.
@@ -120,17 +120,43 @@
     <t xml:space="preserve">On addition of new expense items, graphs are not reflecting the updated numbers.</t>
   </si>
   <si>
-    <t xml:space="preserve">Check whether calculation methods are getting called when the view is shifted to Dashboard.</t>
+    <t xml:space="preserve">Resolved in new version.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Page rendering for mobile need to be fixed.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Resolved</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chart.js and Apex charts need to be rechecked for fixing the graph in mobile layout. Web and mobile layout for the rest of components has been fixed.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Expense table need to be order by purchase Date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Issue in the category expense chart. Maid expense is calculated twice for the month of January. Probably due to the timestamp difference.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Timezone added to the aggregation to resolve the issue.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">With backend server down during login, error pop up is not coming. Probably with wrong credentials it is coming up.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Validate username and email while signing up an user. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rest should be called when the input field is out of focus. If done on key stroke, there will too many calls.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="dd/mm/yy"/>
-    <numFmt numFmtId="166" formatCode="dd/mm/yy"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -213,6 +239,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -227,10 +257,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -242,21 +268,36 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <dxfs count="1">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="00FFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
+  <sheetPr filterMode="true">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E17" activeCellId="0" sqref="E17"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="D21" activeCellId="0" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.77734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.89453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.52"/>
@@ -266,19 +307,19 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
     </row>
@@ -286,7 +327,7 @@
       <c r="A2" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="n">
+      <c r="B2" s="5" t="n">
         <v>44204</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -294,106 +335,112 @@
       </c>
       <c r="D2" s="0" t="s">
         <v>6</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="4" t="n">
+      <c r="B3" s="5" t="n">
         <v>44204</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="0" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="B4" s="4" t="n">
+      <c r="B4" s="5" t="n">
         <v>44204</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D4" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E4" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="B5" s="4" t="n">
+      <c r="B5" s="5" t="n">
         <v>44204</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="B6" s="4" t="n">
+      <c r="B6" s="5" t="n">
         <v>44204</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="B7" s="4" t="n">
+      <c r="B7" s="5" t="n">
         <v>44204</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="B8" s="4" t="n">
+      <c r="B8" s="5" t="n">
         <v>44204</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="35.05" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
         <v>8</v>
       </c>
-      <c r="B9" s="4" t="n">
+      <c r="B9" s="5" t="n">
         <v>44206</v>
       </c>
       <c r="C9" s="1" t="s">
@@ -402,141 +449,228 @@
       <c r="D9" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="E9" s="6" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
         <v>9</v>
       </c>
-      <c r="B10" s="4" t="n">
+      <c r="B10" s="5" t="n">
         <v>44207</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>20</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="B11" s="4" t="n">
+      <c r="B11" s="5" t="n">
         <v>44208</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="23.85" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
         <v>11</v>
       </c>
-      <c r="B12" s="4" t="n">
+      <c r="B12" s="5" t="n">
         <v>44211</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>22</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="E12" s="0" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="23.85" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="B13" s="4" t="n">
+      <c r="B13" s="5" t="n">
         <v>44574</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>24</v>
       </c>
       <c r="D13" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="E13" s="5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="14" customFormat="false" ht="23.85" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="n">
         <v>13</v>
       </c>
-      <c r="B14" s="4" t="n">
+      <c r="B14" s="5" t="n">
         <v>44590</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="n">
         <v>14</v>
       </c>
-      <c r="B15" s="4" t="n">
+      <c r="B15" s="5" t="n">
         <v>44591</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="35.05" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="n">
         <v>15</v>
       </c>
-      <c r="B16" s="4" t="n">
+      <c r="B16" s="5" t="n">
         <v>44606</v>
       </c>
       <c r="C16" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="D16" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="17" customFormat="false" ht="23.85" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="n">
         <v>16</v>
       </c>
-      <c r="B17" s="6" t="n">
+      <c r="B17" s="5" t="n">
         <v>44632</v>
       </c>
       <c r="C17" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E17" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="D17" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="E17" s="5" t="s">
+    </row>
+    <row r="18" customFormat="false" ht="35.05" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" s="5" t="n">
+        <v>45000</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>32</v>
       </c>
+      <c r="D18" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" s="5" t="n">
+        <v>45000</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="35.05" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" s="5" t="n">
+        <v>45001</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D20" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="E20" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" s="5" t="n">
+        <v>45001</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D21" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="23.85" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" s="5" t="n">
+        <v>45002</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D22" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>40</v>
+      </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:E22">
+    <filterColumn colId="3">
+      <filters>
+        <filter val="Open"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>